<commit_message>
add questions and sample
</commit_message>
<xml_diff>
--- a/Interview.xlsx
+++ b/Interview.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26419"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26415"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4B237FB-A16F-49B8-A00E-90134DDD3DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9054D148-3110-4004-A7B7-EE17B70355FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HTML" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="CSS" sheetId="2" r:id="rId3"/>
     <sheet name="JavaScript" sheetId="3" r:id="rId4"/>
     <sheet name="TypeScript" sheetId="4" r:id="rId5"/>
+    <sheet name="Generic" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,31 +33,103 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Question</t>
   </si>
   <si>
-    <t>1. What is HTML and what are its basic features?</t>
-  </si>
-  <si>
-    <t>2. What is the difference between HTML and XHTML?</t>
-  </si>
-  <si>
-    <t>3. What are some common HTML tags and what are their functions?</t>
-  </si>
-  <si>
-    <t>4. What is the difference between an HTML element and an HTML attribute?</t>
-  </si>
-  <si>
-    <t>5. How do you create a link in HTML?</t>
+    <t>1. What is the purpose of the HTML &lt;meta&gt; tag?</t>
+  </si>
+  <si>
+    <t>2. What is the difference between a &lt;div&gt; and a &lt;span&gt; in HTML?</t>
+  </si>
+  <si>
+    <t>3. How do you create a hyperlink in HTML?</t>
+  </si>
+  <si>
+    <t>4. What is the HTML5 data attribute used for?</t>
+  </si>
+  <si>
+    <t>5. How do you create a table in HTML?</t>
+  </si>
+  <si>
+    <t>1. What is JSX in ReactJS?</t>
+  </si>
+  <si>
+    <t>2. What is the difference between state and props in ReactJS?</t>
+  </si>
+  <si>
+    <t>3. How do you handle events in ReactJS?</t>
+  </si>
+  <si>
+    <t>4. How do you pass data between components in ReactJS?</t>
+  </si>
+  <si>
+    <t>5. What is the purpose of ReactJS's virtual DOM?</t>
+  </si>
+  <si>
+    <t>1. What is the box model in CSS?</t>
+  </si>
+  <si>
+    <t>2. What is the difference between padding and margin in CSS?</t>
+  </si>
+  <si>
+    <t>3. How do you center an element horizontally in CSS?</t>
+  </si>
+  <si>
+    <t>4. What is the difference between position: relative and position: absolute in CSS?</t>
+  </si>
+  <si>
+    <t>5. How do you create a responsive layout in CSS?</t>
+  </si>
+  <si>
+    <t>1. What is the difference between null and undefined in JavaScript?</t>
+  </si>
+  <si>
+    <t>2. What is the difference between var, let, and const in JavaScript?</t>
+  </si>
+  <si>
+    <t>3. How do you create a new object in JavaScript?</t>
+  </si>
+  <si>
+    <t>4. What is hoisting in JavaScript?</t>
+  </si>
+  <si>
+    <t>5. How do you handle errors in JavaScript?</t>
+  </si>
+  <si>
+    <t>1. What is TypeScript and how does it differ from JavaScript?</t>
+  </si>
+  <si>
+    <t>2. What are interfaces in TypeScript?</t>
+  </si>
+  <si>
+    <t>3. What is the difference between a class and an interface in TypeScript?</t>
+  </si>
+  <si>
+    <t>4. What are generics in TypeScript?</t>
+  </si>
+  <si>
+    <t>5. How do you define types in TypeScript?</t>
+  </si>
+  <si>
+    <t>Is the Candidate good at Problem Solving ?</t>
+  </si>
+  <si>
+    <t>Was the candidate able to communicate Properly ?</t>
+  </si>
+  <si>
+    <t>Did the Candidate try to understand the question properly ?</t>
+  </si>
+  <si>
+    <t>Is the Candidate open and ready to Learn new Technologies ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +144,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,9 +173,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,9 +493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -463,7 +542,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -478,27 +557,27 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -511,7 +590,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -526,27 +605,27 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -559,7 +638,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -574,27 +653,27 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -606,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10839421-F08F-458E-81B3-AAC9B1C1145C}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -622,27 +701,70 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6177A200-BEE8-41EE-9564-7384F4817E3E}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="59" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>